<commit_message>
Aggiunta la citta' ai nomi degli ospedali
</commit_message>
<xml_diff>
--- a/Dataset_xlsx/centri.xlsx
+++ b/Dataset_xlsx/centri.xlsx
@@ -2,19 +2,19 @@
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
   <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
-  <workbookPr defaultThemeVersion="164011"/>
+  <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\utente\ICon\Dataset_xlsx\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Francesco\ICon\Dataset_xlsx\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="17256" windowHeight="6228"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="17250" windowHeight="6225"/>
   </bookViews>
   <sheets>
     <sheet name="cent" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="162913"/>
+  <calcPr calcId="152511"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -35,24 +35,15 @@
     <t>16.862024</t>
   </si>
   <si>
-    <t>Ospedale Santa Maria</t>
-  </si>
-  <si>
     <t>41.108429</t>
   </si>
   <si>
     <t>16.862101</t>
   </si>
   <si>
-    <t>Ospedale San Paolo</t>
-  </si>
-  <si>
     <t>41.118923</t>
   </si>
   <si>
-    <t>Ospedale Papa Giovanni XXXIII</t>
-  </si>
-  <si>
     <t>41.098381</t>
   </si>
   <si>
@@ -62,37 +53,46 @@
     <t>16.887126</t>
   </si>
   <si>
-    <t>Ospedale Don Tonino Bello</t>
-  </si>
-  <si>
     <t>41.191988</t>
   </si>
   <si>
     <t>16.591516</t>
   </si>
   <si>
-    <t>Ospedale Monsignor Raffaele di Miccoli</t>
-  </si>
-  <si>
     <t>41.313383</t>
   </si>
   <si>
     <t>16.253506</t>
   </si>
   <si>
-    <t>Ospedale IRCSS Saverio De Bellis</t>
-  </si>
-  <si>
     <t>40.883844</t>
   </si>
   <si>
     <t>17.155475</t>
+  </si>
+  <si>
+    <t>Ospedale Santa Maria (Bari)</t>
+  </si>
+  <si>
+    <t>Ospedale San Paolo (Bari)</t>
+  </si>
+  <si>
+    <t>Ospedale Papa Giovanni XXXIII (Bari)</t>
+  </si>
+  <si>
+    <t>Ospedale Don Tonino Bello (Molfetta)</t>
+  </si>
+  <si>
+    <t>Ospedale Monsignor Raffaele di Miccoli (Barletta)</t>
+  </si>
+  <si>
+    <t>Ospedale IRCSS Saverio De Bellis (Castellana)</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <fonts count="1" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -408,17 +408,17 @@
   <dimension ref="A1:D8"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C10" sqref="C10"/>
+      <selection activeCell="B7" sqref="B7"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="2" max="2" width="33.33203125" customWidth="1"/>
-    <col min="3" max="3" width="11.44140625" customWidth="1"/>
-    <col min="4" max="4" width="12.6640625" customWidth="1"/>
+    <col min="2" max="2" width="33.28515625" customWidth="1"/>
+    <col min="3" max="3" width="11.42578125" customWidth="1"/>
+    <col min="4" max="4" width="12.7109375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A1">
         <v>1</v>
       </c>
@@ -432,91 +432,91 @@
         <v>2</v>
       </c>
     </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A2">
         <v>2</v>
       </c>
       <c r="B2" t="s">
+        <v>15</v>
+      </c>
+      <c r="C2" s="1" t="s">
         <v>3</v>
       </c>
-      <c r="C2" s="1" t="s">
+      <c r="D2" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="D2" s="1" t="s">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.3">
+    </row>
+    <row r="3" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A3">
         <v>3</v>
       </c>
       <c r="B3" t="s">
-        <v>6</v>
+        <v>16</v>
       </c>
       <c r="C3" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="D3" s="1" t="s">
         <v>7</v>
       </c>
-      <c r="D3" s="1" t="s">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="4" spans="1:4" x14ac:dyDescent="0.3">
+    </row>
+    <row r="4" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A4">
         <v>4</v>
       </c>
       <c r="B4" t="s">
+        <v>17</v>
+      </c>
+      <c r="C4" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="D4" s="1" t="s">
         <v>8</v>
       </c>
-      <c r="C4" s="1" t="s">
-        <v>9</v>
-      </c>
-      <c r="D4" s="1" t="s">
-        <v>11</v>
-      </c>
-    </row>
-    <row r="5" spans="1:4" x14ac:dyDescent="0.3">
+    </row>
+    <row r="5" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A5">
         <v>5</v>
       </c>
       <c r="B5" t="s">
-        <v>12</v>
+        <v>18</v>
       </c>
       <c r="C5" s="1" t="s">
-        <v>13</v>
+        <v>9</v>
       </c>
       <c r="D5" s="1" t="s">
-        <v>14</v>
-      </c>
-    </row>
-    <row r="6" spans="1:4" x14ac:dyDescent="0.3">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="6" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A6">
         <v>6</v>
       </c>
       <c r="B6" t="s">
-        <v>15</v>
+        <v>19</v>
       </c>
       <c r="C6" s="1" t="s">
-        <v>16</v>
+        <v>11</v>
       </c>
       <c r="D6" s="1" t="s">
-        <v>17</v>
-      </c>
-    </row>
-    <row r="7" spans="1:4" x14ac:dyDescent="0.3">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="7" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A7">
         <v>7</v>
       </c>
       <c r="B7" t="s">
-        <v>18</v>
+        <v>20</v>
       </c>
       <c r="C7" s="1" t="s">
-        <v>19</v>
+        <v>13</v>
       </c>
       <c r="D7" s="1" t="s">
-        <v>20</v>
-      </c>
-    </row>
-    <row r="8" spans="1:4" x14ac:dyDescent="0.3">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="8" spans="1:4" x14ac:dyDescent="0.25">
       <c r="C8" s="1"/>
       <c r="D8" s="1"/>
     </row>

</xml_diff>